<commit_message>
update for FAFSA completion story
</commit_message>
<xml_diff>
--- a/data/FAFSA/output/lunch_status_quantile_fmt.xlsx
+++ b/data/FAFSA/output/lunch_status_quantile_fmt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihodgson/Documents/GitHub/TBTimes_quickturns/data/FAFSA/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2A37C6C3-00E4-1844-AAD1-B6692690928D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A5E823F0-3F66-E144-90FB-8586BBBAADF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30680" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="1"/>
+    <workbookView minimized="1" xWindow="2920" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="lunch_status_quantile" sheetId="1" r:id="rId1"/>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E31" sqref="E31:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,16 +1284,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A2, lunch_status_quantile!$B:$B, 2023)</f>
-        <v>0.31867030965391602</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A2, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>31.867030965391603</v>
       </c>
       <c r="C2">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A2, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.17918874315990599</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A2, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>17.9188743159906</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>0.13948156649401003</v>
+        <v>13.948156649401003</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1301,16 +1301,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A3, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.33216656608328299</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A3, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>33.2166566083283</v>
       </c>
       <c r="C3">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A3, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.19975310093468901</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A3, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>19.975310093468902</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D11" si="0">B3-C3</f>
-        <v>0.13241346514859398</v>
+        <v>13.241346514859398</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,16 +1318,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A4, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.34680095476509198</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A4, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>34.680095476509202</v>
       </c>
       <c r="C4">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A4, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.21099038625632799</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A4, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>21.099038625632797</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.135810568508764</v>
+        <v>13.581056850876404</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1335,16 +1335,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A5, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.35952874158467102</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A5, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>35.952874158467104</v>
       </c>
       <c r="C5">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A5, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.22745047759471701</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A5, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>22.745047759471699</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.13207826398995401</v>
+        <v>13.207826398995405</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1352,16 +1352,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A6, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.352722640908608</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A6, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>35.272264090860801</v>
       </c>
       <c r="C6">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A6, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.223637470821069</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A6, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>22.363747082106901</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.129085170087539</v>
+        <v>12.908517008753901</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1369,16 +1369,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A7, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.38736223365172601</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A7, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>38.736223365172599</v>
       </c>
       <c r="C7">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A7, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.26560684237437798</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A7, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>26.560684237437798</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.12175539127734802</v>
+        <v>12.175539127734801</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1386,16 +1386,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A8, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.38766134325092899</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A8, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>38.766134325092899</v>
       </c>
       <c r="C8">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A8, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.259054406211774</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A8, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>25.905440621177402</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.12860693703915499</v>
+        <v>12.860693703915498</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1403,16 +1403,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A9, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.427698574338085</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A9, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>42.769857433808497</v>
       </c>
       <c r="C9">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A9, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.284650470073536</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A9, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>28.465047007353601</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.143048104264549</v>
+        <v>14.304810426454896</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,16 +1420,16 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A10, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.46563348628148699</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A10, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>46.563348628148695</v>
       </c>
       <c r="C10">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A10, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.31839776432230998</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A10, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>31.839776432230998</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.147235721959177</v>
+        <v>14.723572195917697</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1437,16 +1437,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <f>SUMIFS(lunch_status_quantile!C:C, lunch_status_quantile!A:A, Sheet1!A11, lunch_status_quantile!B:B, 2023)</f>
-        <v>0.48515111695137902</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A11, lunch_status_quantile!$B:$B, 2023)*100</f>
+        <v>48.515111695137904</v>
       </c>
       <c r="C11">
-        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A11, lunch_status_quantile!$B:$B, 2024)</f>
-        <v>0.34155019059720398</v>
+        <f>SUMIFS(lunch_status_quantile!$C:$C, lunch_status_quantile!$A:$A, Sheet1!$A11, lunch_status_quantile!$B:$B, 2024)*100</f>
+        <v>34.155019059720395</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.14360092635417504</v>
+        <v>14.360092635417509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>